<commit_message>
errori ipynb luca è il migliore
</commit_message>
<xml_diff>
--- a/20240523spettrometria/dati_sottrometria.xlsx
+++ b/20240523spettrometria/dati_sottrometria.xlsx
@@ -3,11 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ERRORI" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="PRISMA carlona" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="PRISMA" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="RETICOLO" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr/>
 </workbook>
@@ -1481,4 +1482,20 @@
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cheppalle è ancora mercurio
</commit_message>
<xml_diff>
--- a/20240523spettrometria/dati_sottrometria.xlsx
+++ b/20240523spettrometria/dati_sottrometria.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ERRORI" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,14 +11,15 @@
     <sheet name="luce misteriosa" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="reticolo" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="alpha" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="deltam" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="deltam_prisma" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="composto_misterioso_prisma" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t xml:space="preserve">SARA deg</t>
   </si>
@@ -153,6 +154,81 @@
   </si>
   <si>
     <t>FACCIA2prim</t>
+  </si>
+  <si>
+    <t>gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROSSO deg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROSSO prim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACQUA deg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACQUA prim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIOLA2 deg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIOLA2 prim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIOLA 1 deg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIOLA 1 prim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nota: bisogna fare 360-angolo letto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POCO VISIBILE</t>
+  </si>
+  <si>
+    <t>VISIBIISSIMO</t>
+  </si>
+  <si>
+    <t>VISIBILISSIMO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gas ignoto</t>
+  </si>
+  <si>
+    <t>GIALLOdeg</t>
+  </si>
+  <si>
+    <t>GIALLOprim</t>
+  </si>
+  <si>
+    <t>VERDEdeg</t>
+  </si>
+  <si>
+    <t>VERDEprim</t>
+  </si>
+  <si>
+    <t>BLUdeg</t>
+  </si>
+  <si>
+    <t>BLUprim</t>
+  </si>
+  <si>
+    <t>VIOLA2deg</t>
+  </si>
+  <si>
+    <t>VIOLA2prim</t>
+  </si>
+  <si>
+    <t>ACQUAdeg</t>
+  </si>
+  <si>
+    <t>ACQUAprim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(quello più vicino al verde)</t>
   </si>
 </sst>
 </file>
@@ -192,7 +268,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,6 +359,30 @@
         <bgColor rgb="FFEE30FF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="2"/>
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6EEEFF"/>
+        <bgColor rgb="FF6EEEFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBB00FF"/>
+        <bgColor rgb="FFBB00FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="5"/>
+        <bgColor indexed="5"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -302,7 +402,7 @@
     <xf fontId="2" fillId="6" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="30">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="3" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf fontId="3" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -323,6 +423,18 @@
     <xf fontId="4" fillId="14" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf fontId="4" fillId="15" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="16" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="17" borderId="0" numFmtId="0" xfId="2" applyFill="1"/>
+    <xf fontId="4" fillId="18" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf fontId="4" fillId="15" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="19" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="15" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="17" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2122,8 +2234,252 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="9.3828125"/>
+    <col bestFit="1" min="2" max="2" width="10.7109375"/>
+    <col bestFit="1" min="3" max="3" width="11.19140625"/>
+    <col customWidth="1" min="5" max="5" width="13.28125"/>
+    <col customWidth="1" min="6" max="9" width="11.8515625"/>
+    <col bestFit="1" min="12" max="12" width="10.61328125"/>
+    <col bestFit="1" min="13" max="13" width="11.57421875"/>
+    <col customWidth="1" min="14" max="14" width="12.421875"/>
+    <col bestFit="1" customWidth="1" min="15" max="15" width="12.04296875"/>
+    <col customWidth="1" min="16" max="16" width="11.28125"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="22"/>
+      <c r="Q1"/>
+      <c r="R1"/>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>311</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>311</v>
+      </c>
+      <c r="E2">
+        <v>40</v>
+      </c>
+      <c r="F2">
+        <v>311</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="17">
+        <v>310</v>
+      </c>
+      <c r="I2" s="17">
+        <v>40</v>
+      </c>
+      <c r="J2">
+        <v>309</v>
+      </c>
+      <c r="K2">
+        <v>30</v>
+      </c>
+      <c r="L2" s="17">
+        <v>308</v>
+      </c>
+      <c r="M2" s="17">
+        <v>40</v>
+      </c>
+      <c r="N2">
+        <v>308</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25"/>
+    <row r="4" ht="14.25">
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="10.57421875"/>
+    <col customWidth="1" min="2" max="2" width="12.28125"/>
+    <col customWidth="1" min="3" max="3" width="12.421875"/>
+    <col customWidth="1" min="9" max="9" width="9.8515625"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2"/>
+      <c r="B2">
+        <v>311</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>311</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>309</v>
+      </c>
+      <c r="G2">
+        <v>35</v>
+      </c>
+      <c r="H2">
+        <v>308</v>
+      </c>
+      <c r="I2">
+        <v>45</v>
+      </c>
+      <c r="J2">
+        <v>310</v>
+      </c>
+      <c r="K2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25"/>
+    <row r="5" ht="14.25"/>
+    <row r="6" ht="14.25"/>
+    <row r="7" ht="14.25"/>
+    <row r="8" ht="14.25"/>
+    <row r="9" ht="14.25"/>
+    <row r="10" ht="14.25"/>
+    <row r="11" ht="14.25"/>
+  </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>

</xml_diff>

<commit_message>
gas ignoto con reticolo, prima della ricalibrazione
</commit_message>
<xml_diff>
--- a/20240523spettrometria/dati_sottrometria.xlsx
+++ b/20240523spettrometria/dati_sottrometria.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="8"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="ERRORI" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,13 +15,15 @@
     <sheet name="composto_misterioso_prisma" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="prismaNA" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="prismaIgnoto" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="PRISMA EXTRA" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="prisma incognito 2" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
   <si>
     <t xml:space="preserve">SARA deg</t>
   </si>
@@ -308,14 +310,65 @@
     <t xml:space="preserve">gas ignoto</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t xml:space="preserve">(si vede anche la frangia blu del 4 ordine)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(abbiamo preso l'acqua più a sinistra)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(in caso di doppia riga prendiamo quella piu a sinistra)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RIPRESA DATI SULL'ANGOLO MINIMA DEVIAZIONE Hg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acqua: pesa quella a sx (più grossa)</t>
+  </si>
+  <si>
+    <t>ROSSOdeg</t>
+  </si>
+  <si>
+    <t>ROSSOprim</t>
+  </si>
+  <si>
+    <t>AZZURROdeg</t>
+  </si>
+  <si>
+    <t>AZZURROprim</t>
+  </si>
+  <si>
+    <t>PRISMA</t>
+  </si>
+  <si>
+    <t>-n1</t>
+  </si>
+  <si>
+    <t>RETICOLOn1</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>prim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RETICOLO n2</t>
+  </si>
+  <si>
+    <t>RETICOLO-n1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POTREBBE ESSERE STATO CORRETTO NELLA DIREZIONE SBAGLIATA (GIRATO DI UN GRADO)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RETICOLO -n2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -335,6 +388,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11.000000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -347,8 +406,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color theme="1" tint="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="21">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,6 +455,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor theme="7" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -469,8 +541,14 @@
         <bgColor rgb="FF00B050"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF0070C0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -478,8 +556,21 @@
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="none"/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="0" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
@@ -487,52 +578,70 @@
     <xf fontId="1" fillId="5" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="2" fillId="6" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="3" fillId="8" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="47">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="3" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf fontId="3" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf fontId="3" fillId="4" borderId="0" numFmtId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf fontId="4" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf fontId="4" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf fontId="4" fillId="4" borderId="0" numFmtId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFill="1"/>
     <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFill="1"/>
     <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="3" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="6" applyFill="1"/>
-    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="2" applyFill="1"/>
-    <xf fontId="4" fillId="10" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf fontId="4" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="6" applyFill="1"/>
+    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="2" applyFill="1"/>
+    <xf fontId="5" fillId="11" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf fontId="5" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="4" fillId="12" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf fontId="4" fillId="13" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf fontId="4" fillId="14" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf fontId="4" fillId="15" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf fontId="5" fillId="13" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf fontId="5" fillId="14" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf fontId="5" fillId="15" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf fontId="5" fillId="16" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="17" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="18" borderId="0" numFmtId="0" xfId="2" applyFill="1"/>
+    <xf fontId="5" fillId="19" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf fontId="5" fillId="16" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="20" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="13" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="16" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="17" borderId="0" numFmtId="0" xfId="2" applyFill="1"/>
-    <xf fontId="4" fillId="18" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf fontId="4" fillId="15" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="19" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="15" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="17" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="18" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="19" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="19" borderId="0" numFmtId="0" xfId="0" applyFill="1">
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="20" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="20" borderId="0" numFmtId="0" xfId="0" applyFill="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="20" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="21" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="22" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="22" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="18" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="4" fillId="17" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="4" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="6" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="4" fillId="18" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="4" fillId="22" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="3" fillId="8" borderId="0" numFmtId="0" xfId="7" applyFont="1" applyFill="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
     <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
@@ -540,6 +649,7 @@
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Good" xfId="5" builtinId="26"/>
     <cellStyle name="20% - Accent4" xfId="6" builtinId="42"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1310,6 +1420,374 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="O3" s="21"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="12">
+        <v>312</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0</v>
+      </c>
+      <c r="C4" s="12">
+        <v>311</v>
+      </c>
+      <c r="D4" s="12">
+        <v>40</v>
+      </c>
+      <c r="E4" s="12">
+        <v>311</v>
+      </c>
+      <c r="F4" s="12">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>310</v>
+      </c>
+      <c r="H4">
+        <v>40</v>
+      </c>
+      <c r="I4" s="12">
+        <v>309</v>
+      </c>
+      <c r="J4" s="12">
+        <v>35</v>
+      </c>
+      <c r="K4">
+        <v>308</v>
+      </c>
+      <c r="L4">
+        <v>40</v>
+      </c>
+      <c r="M4" s="12">
+        <v>308</v>
+      </c>
+      <c r="N4" s="12">
+        <v>5</v>
+      </c>
+      <c r="O4" s="12"/>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>312</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>311</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>311</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>310</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+      <c r="I5">
+        <v>309</v>
+      </c>
+      <c r="J5">
+        <v>30</v>
+      </c>
+      <c r="K5">
+        <v>308</v>
+      </c>
+      <c r="L5">
+        <v>44</v>
+      </c>
+      <c r="M5">
+        <v>308</v>
+      </c>
+      <c r="N5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="G6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="15.00390625"/>
+    <col customWidth="1" min="2" max="2" width="13.421875"/>
+    <col customWidth="1" min="3" max="3" width="11.421875"/>
+    <col customWidth="1" min="4" max="4" width="11.28125"/>
+    <col customWidth="1" min="5" max="5" width="12.28125"/>
+    <col customWidth="1" min="6" max="6" width="11.8515625"/>
+    <col customWidth="1" min="7" max="7" width="13.7109375"/>
+    <col customWidth="1" min="8" max="8" width="14.28125"/>
+    <col customWidth="1" min="11" max="11" width="13.7109375"/>
+    <col customWidth="1" min="12" max="12" width="31.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2">
+        <v>312</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>311</v>
+      </c>
+      <c r="D2">
+        <v>40</v>
+      </c>
+      <c r="E2">
+        <v>311</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>310</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2">
+        <v>310</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2" s="29"/>
+      <c r="M2" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" s="43"/>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="C3" s="12">
+        <v>10</v>
+      </c>
+      <c r="D3" s="12">
+        <v>49</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="L3" s="29"/>
+      <c r="M3" t="s">
+        <v>107</v>
+      </c>
+      <c r="N3" t="s">
+        <v>108</v>
+      </c>
+      <c r="O3" t="s">
+        <v>107</v>
+      </c>
+      <c r="P3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="12">
+        <v>21</v>
+      </c>
+      <c r="D4" s="12">
+        <v>24</v>
+      </c>
+      <c r="K4" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="L4" s="45"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5">
+        <v>349</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5" s="46">
+        <v>350</v>
+      </c>
+      <c r="D5" s="12">
+        <v>38</v>
+      </c>
+      <c r="E5">
+        <v>351</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="L5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M5" s="12">
+        <v>9</v>
+      </c>
+      <c r="N5" s="12">
+        <v>49</v>
+      </c>
+      <c r="O5" s="12">
+        <v>349</v>
+      </c>
+      <c r="P5" s="12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="C6">
+        <v>340</v>
+      </c>
+      <c r="D6">
+        <v>22</v>
+      </c>
+      <c r="K6" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+  </mergeCells>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
@@ -2583,7 +3061,7 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2839,15 +3317,217 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="14.25">
       <c r="A1" t="s">
         <v>94</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="B2" s="34">
+        <v>352</v>
+      </c>
+      <c r="C2" s="35">
+        <v>20</v>
+      </c>
+      <c r="D2" s="35">
+        <v>344</v>
+      </c>
+      <c r="E2" s="35">
+        <v>30</v>
+      </c>
+      <c r="F2" s="35">
+        <v>336</v>
+      </c>
+      <c r="G2" s="35">
+        <v>30</v>
+      </c>
+      <c r="H2"/>
+      <c r="I2" s="32" t="s">
         <v>95</v>
       </c>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="B3" s="26">
+        <v>351</v>
+      </c>
+      <c r="C3" s="26">
+        <v>15</v>
+      </c>
+      <c r="D3" s="26">
+        <v>342</v>
+      </c>
+      <c r="E3" s="26">
+        <v>33</v>
+      </c>
+      <c r="F3" s="26">
+        <v>332</v>
+      </c>
+      <c r="G3" s="36">
+        <v>56</v>
+      </c>
+      <c r="H3"/>
+      <c r="I3" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="B4" s="23">
+        <v>350</v>
+      </c>
+      <c r="C4" s="23">
+        <v>20</v>
+      </c>
+      <c r="D4" s="23">
+        <v>340</v>
+      </c>
+      <c r="E4" s="23">
+        <v>30</v>
+      </c>
+      <c r="F4" s="23">
+        <v>330</v>
+      </c>
+      <c r="G4" s="23">
+        <v>2</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="B5" s="37">
+        <v>349</v>
+      </c>
+      <c r="C5" s="37">
+        <v>51</v>
+      </c>
+      <c r="D5" s="37">
+        <v>339</v>
+      </c>
+      <c r="E5" s="37">
+        <v>20</v>
+      </c>
+      <c r="F5" s="37">
+        <v>328</v>
+      </c>
+      <c r="G5" s="37">
+        <v>0</v>
+      </c>
+      <c r="H5"/>
+      <c r="I5" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="F8"/>
+      <c r="G8" s="32"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="N11"/>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="N12"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="N13"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="N14"/>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="N15"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
da fare i colori delle linee hg
</commit_message>
<xml_diff>
--- a/20240523spettrometria/dati_sottrometria.xlsx
+++ b/20240523spettrometria/dati_sottrometria.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ERRORI" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,18 +11,17 @@
     <sheet name="alpha" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="composto_misterioso_prisma" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="reticolo300" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Reticolo 300 ma mejo" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="reticoloIgnoto" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="PRISMA EXTRA" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="incognito 2" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="reticolo600" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="reticoloIgnoto" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="PRISMA Hg" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="incognito 2" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="reticolo600" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t xml:space="preserve">SARA deg</t>
   </si>
@@ -246,13 +245,25 @@
     <t xml:space="preserve">RIPRESA DATI SULL'ANGOLO MINIMA DEVIAZIONE Hg</t>
   </si>
   <si>
-    <t xml:space="preserve">POCO VISIBILE</t>
-  </si>
-  <si>
-    <t>VISIBIISSIMO</t>
+    <t xml:space="preserve">ROSSO:poco visibile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIALLO: molto visibile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VERDE: molto visibile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACQUA: meno ma visibile</t>
   </si>
   <si>
     <t xml:space="preserve">acqua: pesa quella a sx (più grossa)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLU: molto visibile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIOLA12: poco visibili</t>
   </si>
   <si>
     <t>ROSSOdeg</t>
@@ -510,7 +521,7 @@
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="3" fillId="8" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="4" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf fontId="4" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -547,6 +558,7 @@
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="4" fillId="19" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="4" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="6" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1335,133 +1347,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData>
-    <row r="1" ht="14.25">
-      <c r="A1" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" ht="14.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="21">
-        <v>343</v>
-      </c>
-      <c r="C2" s="21">
-        <v>0</v>
-      </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-    </row>
-    <row r="3" ht="14.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="16">
-        <v>342</v>
-      </c>
-      <c r="C3" s="16">
-        <v>45</v>
-      </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-    </row>
-    <row r="4" ht="14.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="13">
-        <v>340</v>
-      </c>
-      <c r="C4" s="13">
-        <v>10</v>
-      </c>
-      <c r="D4" s="13">
-        <v>317</v>
-      </c>
-      <c r="E4" s="13">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="23">
-        <v>339</v>
-      </c>
-      <c r="C5" s="23">
-        <v>28</v>
-      </c>
-      <c r="D5" s="23">
-        <v>315</v>
-      </c>
-      <c r="E5" s="23">
-        <v>1</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25">
-      <c r="B6" s="24">
-        <v>338</v>
-      </c>
-      <c r="C6" s="24">
-        <v>30</v>
-      </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-    </row>
-    <row r="7" ht="14.25"/>
-    <row r="8" ht="14.25"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F2:N3"/>
-  </mergeCells>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
@@ -2318,7 +2203,132 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="B2" s="21">
+        <v>352</v>
+      </c>
+      <c r="C2" s="21">
+        <v>20</v>
+      </c>
+      <c r="D2" s="21">
+        <v>344</v>
+      </c>
+      <c r="E2" s="21">
+        <v>30</v>
+      </c>
+      <c r="F2" s="21">
+        <v>336</v>
+      </c>
+      <c r="G2" s="21">
+        <v>30</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="B3" s="16">
+        <v>351</v>
+      </c>
+      <c r="C3" s="16">
+        <v>15</v>
+      </c>
+      <c r="D3" s="16">
+        <v>342</v>
+      </c>
+      <c r="E3" s="16">
+        <v>33</v>
+      </c>
+      <c r="F3" s="16">
+        <v>332</v>
+      </c>
+      <c r="G3" s="22">
+        <v>56</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="B4" s="13">
+        <v>350</v>
+      </c>
+      <c r="C4" s="13">
+        <v>20</v>
+      </c>
+      <c r="D4" s="13">
+        <v>340</v>
+      </c>
+      <c r="E4" s="13">
+        <v>30</v>
+      </c>
+      <c r="F4" s="13">
+        <v>330</v>
+      </c>
+      <c r="G4" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="B5" s="23">
+        <v>349</v>
+      </c>
+      <c r="C5" s="23">
+        <v>51</v>
+      </c>
+      <c r="D5" s="23">
+        <v>339</v>
+      </c>
+      <c r="E5" s="23">
+        <v>20</v>
+      </c>
+      <c r="F5" s="23">
+        <v>328</v>
+      </c>
+      <c r="G5" s="23">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25"/>
+    <row r="7" ht="14.25"/>
+    <row r="8" ht="14.25">
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" ht="14.25"/>
+    <row r="10" ht="14.25"/>
+    <row r="11" ht="14.25"/>
+    <row r="12" ht="14.25"/>
+    <row r="13" ht="14.25"/>
+    <row r="14" ht="14.25"/>
+    <row r="15" ht="14.25"/>
+  </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
@@ -2335,130 +2345,244 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" ht="14.25">
-      <c r="A1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="18" t="s">
+    <row r="1">
+      <c r="A1" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+      <c r="R1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="28">
+        <v>311</v>
+      </c>
+      <c r="B2" s="28">
+        <v>50</v>
+      </c>
+      <c r="C2" s="28">
+        <v>311</v>
+      </c>
+      <c r="D2" s="28">
+        <v>40</v>
+      </c>
+      <c r="E2" s="28">
+        <v>311</v>
+      </c>
+      <c r="F2" s="28">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>310</v>
+      </c>
+      <c r="H2">
+        <v>40</v>
+      </c>
+      <c r="I2" s="28">
+        <v>309</v>
+      </c>
+      <c r="J2" s="28">
+        <v>30</v>
+      </c>
+      <c r="K2">
+        <v>308</v>
+      </c>
+      <c r="L2">
+        <v>40</v>
+      </c>
+      <c r="M2" s="28">
+        <v>308</v>
+      </c>
+      <c r="N2" s="28">
+        <v>0</v>
+      </c>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="29"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="28">
+        <v>312</v>
+      </c>
+      <c r="B3" s="28">
+        <v>0</v>
+      </c>
+      <c r="C3" s="28">
+        <v>311</v>
+      </c>
+      <c r="D3" s="28">
+        <v>40</v>
+      </c>
+      <c r="E3" s="28">
+        <v>311</v>
+      </c>
+      <c r="F3" s="28">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>310</v>
+      </c>
+      <c r="H3">
+        <v>40</v>
+      </c>
+      <c r="I3" s="28">
+        <v>309</v>
+      </c>
+      <c r="J3" s="28">
+        <v>35</v>
+      </c>
+      <c r="K3">
+        <v>308</v>
+      </c>
+      <c r="L3">
+        <v>40</v>
+      </c>
+      <c r="M3" s="28">
+        <v>308</v>
+      </c>
+      <c r="N3" s="28">
+        <v>5</v>
+      </c>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>312</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>311</v>
+      </c>
+      <c r="D4">
+        <v>40</v>
+      </c>
+      <c r="E4">
+        <v>311</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>310</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4">
+        <v>309</v>
+      </c>
+      <c r="J4">
+        <v>30</v>
+      </c>
+      <c r="K4">
+        <v>308</v>
+      </c>
+      <c r="L4">
+        <v>44</v>
+      </c>
+      <c r="M4">
+        <v>308</v>
+      </c>
+      <c r="N4">
         <v>38</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" ht="14.25">
-      <c r="B2" s="21">
-        <v>352</v>
-      </c>
-      <c r="C2" s="21">
-        <v>20</v>
-      </c>
-      <c r="D2" s="21">
-        <v>344</v>
-      </c>
-      <c r="E2" s="21">
-        <v>30</v>
-      </c>
-      <c r="F2" s="21">
-        <v>336</v>
-      </c>
-      <c r="G2" s="21">
-        <v>30</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25">
-      <c r="B3" s="16">
-        <v>351</v>
-      </c>
-      <c r="C3" s="16">
-        <v>15</v>
-      </c>
-      <c r="D3" s="16">
-        <v>342</v>
-      </c>
-      <c r="E3" s="16">
-        <v>33</v>
-      </c>
-      <c r="F3" s="16">
-        <v>332</v>
-      </c>
-      <c r="G3" s="22">
-        <v>56</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25">
-      <c r="B4" s="13">
-        <v>350</v>
-      </c>
-      <c r="C4" s="13">
-        <v>20</v>
-      </c>
-      <c r="D4" s="13">
-        <v>340</v>
-      </c>
-      <c r="E4" s="13">
-        <v>30</v>
-      </c>
-      <c r="F4" s="13">
-        <v>330</v>
-      </c>
-      <c r="G4" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25">
-      <c r="B5" s="23">
-        <v>349</v>
-      </c>
-      <c r="C5" s="23">
-        <v>51</v>
-      </c>
-      <c r="D5" s="23">
-        <v>339</v>
-      </c>
-      <c r="E5" s="23">
-        <v>20</v>
-      </c>
-      <c r="F5" s="23">
-        <v>328</v>
-      </c>
-      <c r="G5" s="23">
-        <v>0</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25"/>
-    <row r="7" ht="14.25"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="R6" t="s">
+        <v>77</v>
+      </c>
+      <c r="T6" s="28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="R7" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="8" ht="14.25">
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" ht="14.25"/>
-    <row r="10" ht="14.25"/>
-    <row r="11" ht="14.25"/>
-    <row r="12" ht="14.25"/>
-    <row r="13" ht="14.25"/>
-    <row r="14" ht="14.25"/>
-    <row r="15" ht="14.25"/>
+      <c r="R8" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -2468,236 +2592,6 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="M1" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="N1" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="O1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="28">
-        <v>311</v>
-      </c>
-      <c r="B2" s="28">
-        <v>50</v>
-      </c>
-      <c r="C2" s="28">
-        <v>311</v>
-      </c>
-      <c r="D2" s="28">
-        <v>40</v>
-      </c>
-      <c r="E2" s="28">
-        <v>311</v>
-      </c>
-      <c r="F2" s="28">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>310</v>
-      </c>
-      <c r="H2">
-        <v>40</v>
-      </c>
-      <c r="I2" s="28">
-        <v>309</v>
-      </c>
-      <c r="J2" s="28">
-        <v>30</v>
-      </c>
-      <c r="K2">
-        <v>308</v>
-      </c>
-      <c r="L2">
-        <v>40</v>
-      </c>
-      <c r="M2" s="28">
-        <v>308</v>
-      </c>
-      <c r="N2" s="28">
-        <v>0</v>
-      </c>
-      <c r="O2" s="29"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="28">
-        <v>312</v>
-      </c>
-      <c r="B3" s="28">
-        <v>0</v>
-      </c>
-      <c r="C3" s="28">
-        <v>311</v>
-      </c>
-      <c r="D3" s="28">
-        <v>40</v>
-      </c>
-      <c r="E3" s="28">
-        <v>311</v>
-      </c>
-      <c r="F3" s="28">
-        <v>20</v>
-      </c>
-      <c r="G3">
-        <v>310</v>
-      </c>
-      <c r="H3">
-        <v>40</v>
-      </c>
-      <c r="I3" s="28">
-        <v>309</v>
-      </c>
-      <c r="J3" s="28">
-        <v>35</v>
-      </c>
-      <c r="K3">
-        <v>308</v>
-      </c>
-      <c r="L3">
-        <v>40</v>
-      </c>
-      <c r="M3" s="28">
-        <v>308</v>
-      </c>
-      <c r="N3" s="28">
-        <v>5</v>
-      </c>
-      <c r="O3" s="28"/>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>312</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>311</v>
-      </c>
-      <c r="D4">
-        <v>40</v>
-      </c>
-      <c r="E4">
-        <v>311</v>
-      </c>
-      <c r="F4">
-        <v>20</v>
-      </c>
-      <c r="G4">
-        <v>310</v>
-      </c>
-      <c r="H4">
-        <v>30</v>
-      </c>
-      <c r="I4">
-        <v>309</v>
-      </c>
-      <c r="J4">
-        <v>30</v>
-      </c>
-      <c r="K4">
-        <v>308</v>
-      </c>
-      <c r="L4">
-        <v>44</v>
-      </c>
-      <c r="M4">
-        <v>308</v>
-      </c>
-      <c r="N4">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-    </row>
-    <row r="6">
-      <c r="G6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7"/>
-  </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">
@@ -2719,42 +2613,42 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="31" t="s">
+      <c r="A1" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="I1" s="34" t="s">
+      <c r="G1" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
     </row>
     <row r="2" ht="14.25">
       <c r="A2">
@@ -2788,19 +2682,19 @@
         <v>6</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="M2" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="P2" s="35"/>
+        <v>86</v>
+      </c>
+      <c r="M2" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="P2" s="36"/>
     </row>
     <row r="3" ht="14.25">
       <c r="A3">
@@ -2834,20 +2728,20 @@
         <v>56</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="L3" s="18"/>
       <c r="M3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="N3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="O3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="P3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" ht="14.25">
@@ -2882,10 +2776,10 @@
         <v>20</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="L4" s="18" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="M4">
         <v>20</v>
@@ -2923,4 +2817,131 @@
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="28"/>
+      <c r="B2" s="21">
+        <v>343</v>
+      </c>
+      <c r="C2" s="21">
+        <v>0</v>
+      </c>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="28"/>
+      <c r="B3" s="16">
+        <v>342</v>
+      </c>
+      <c r="C3" s="16">
+        <v>45</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="13">
+        <v>340</v>
+      </c>
+      <c r="C4" s="13">
+        <v>10</v>
+      </c>
+      <c r="D4" s="13">
+        <v>317</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="28"/>
+      <c r="B5" s="23">
+        <v>339</v>
+      </c>
+      <c r="C5" s="23">
+        <v>28</v>
+      </c>
+      <c r="D5" s="23">
+        <v>315</v>
+      </c>
+      <c r="E5" s="23">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="B6" s="24">
+        <v>338</v>
+      </c>
+      <c r="C6" s="24">
+        <v>30</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" ht="14.25"/>
+    <row r="8" ht="14.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:N3"/>
+  </mergeCells>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>